<commit_message>
test min_cons=4 untuk eksperimen final
</commit_message>
<xml_diff>
--- a/3 Base-line system (Makarand 2018)/Matching with Unified Algorithm/Hasil eksperimen/Tabel Hasil Eksperimen Final.xlsx
+++ b/3 Base-line system (Makarand 2018)/Matching with Unified Algorithm/Hasil eksperimen/Tabel Hasil Eksperimen Final.xlsx
@@ -401,22 +401,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -745,37 +745,37 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="14"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="18"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="16"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
@@ -919,37 +919,37 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="14"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="18"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="16"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="8" t="s">
         <v>14</v>
       </c>
@@ -1217,18 +1217,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G10:M10"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="G2:M2"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G10:M10"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Eksperimen ulang tanpa FSD SS beres
</commit_message>
<xml_diff>
--- a/3 Base-line system (Makarand 2018)/Matching with Unified Algorithm/Hasil eksperimen/Tabel Hasil Eksperimen Final.xlsx
+++ b/3 Base-line system (Makarand 2018)/Matching with Unified Algorithm/Hasil eksperimen/Tabel Hasil Eksperimen Final.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="69">
   <si>
     <t>No</t>
   </si>
@@ -46,9 +46,6 @@
     <t>FSD-SS</t>
   </si>
   <si>
-    <t>Avg Time (s)</t>
-  </si>
-  <si>
     <t>Pencocokan</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>0.72</t>
   </si>
   <si>
-    <t>0.217</t>
-  </si>
-  <si>
     <t>0.27</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>0.63</t>
   </si>
   <si>
-    <t>0.191</t>
-  </si>
-  <si>
     <t>0.30</t>
   </si>
   <si>
@@ -130,15 +121,9 @@
     <t>0.71</t>
   </si>
   <si>
-    <t>0.981</t>
-  </si>
-  <si>
     <t>0.11</t>
   </si>
   <si>
-    <t>0.793</t>
-  </si>
-  <si>
     <t>0.22</t>
   </si>
   <si>
@@ -200,6 +185,42 @@
   </si>
   <si>
     <t>0.219</t>
+  </si>
+  <si>
+    <t>0.808</t>
+  </si>
+  <si>
+    <t>0.198</t>
+  </si>
+  <si>
+    <t>0.212</t>
+  </si>
+  <si>
+    <t>Ekstraksi melodi</t>
+  </si>
+  <si>
+    <t>15.79</t>
+  </si>
+  <si>
+    <t>15.69</t>
+  </si>
+  <si>
+    <t>0.993</t>
+  </si>
+  <si>
+    <t>0.229</t>
+  </si>
+  <si>
+    <t>0.151</t>
+  </si>
+  <si>
+    <t>0.288</t>
+  </si>
+  <si>
+    <t>0.237</t>
+  </si>
+  <si>
+    <t>0.122</t>
   </si>
 </sst>
 </file>
@@ -249,7 +270,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -396,18 +417,46 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -428,38 +477,62 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -765,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,70 +850,81 @@
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="18"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="17"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="8" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="13"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -856,30 +940,36 @@
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
+      <c r="F4" s="20"/>
+      <c r="G4" s="3">
         <v>4431</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>27</v>
+      <c r="M4" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -892,30 +982,36 @@
       <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2">
+      <c r="F5" s="20"/>
+      <c r="G5" s="3">
         <v>4383</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>33</v>
+      <c r="M5" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="26">
+        <v>10145</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -928,30 +1024,36 @@
       <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
+      <c r="F6" s="20"/>
+      <c r="G6" s="3">
         <v>4426</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="J6" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>55</v>
+        <v>34</v>
+      </c>
+      <c r="M6" s="26">
+        <v>1104</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>4</v>
       </c>
@@ -964,85 +1066,99 @@
       <c r="E7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6">
+      <c r="F7" s="21"/>
+      <c r="G7" s="5">
         <v>4408</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" s="25">
+        <v>9806</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="17"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="13"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>61</v>
+      <c r="O11" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="18"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1058,30 +1174,36 @@
       <c r="E12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2">
+      <c r="F12" s="20"/>
+      <c r="G12" s="3">
         <v>759</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M12" s="11">
-        <v>7571</v>
+        <v>36</v>
+      </c>
+      <c r="M12" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="O12" s="9">
+        <v>8094</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>2</v>
       </c>
@@ -1094,35 +1216,41 @@
       <c r="E13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2">
+      <c r="F13" s="20"/>
+      <c r="G13" s="3">
         <v>759</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M13" s="11">
-        <v>6448</v>
+      <c r="M13" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="N13" s="26">
+        <v>16198</v>
+      </c>
+      <c r="O13" s="9">
+        <v>6006</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
@@ -1130,37 +1258,41 @@
       <c r="E14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="2">
-        <v>340</v>
+      <c r="F14" s="20"/>
+      <c r="G14" s="3">
+        <v>759</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M14" s="11" t="s">
-        <v>38</v>
+        <v>47</v>
+      </c>
+      <c r="M14" s="26">
+        <v>1277</v>
+      </c>
+      <c r="N14" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O14" s="9">
+        <v>7450</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
@@ -1168,37 +1300,41 @@
       <c r="E15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="2">
-        <v>340</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>23</v>
+      <c r="F15" s="20"/>
+      <c r="G15" s="3">
+        <v>759</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M15" s="11" t="s">
-        <v>40</v>
+        <v>21</v>
+      </c>
+      <c r="M15" s="26">
+        <v>1201</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="O15" s="9">
+        <v>5424</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
@@ -1206,35 +1342,43 @@
       <c r="E16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2">
-        <v>759</v>
+      <c r="F16" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="3">
+        <v>340</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="M16" s="11">
-        <v>7450</v>
+        <v>34</v>
+      </c>
+      <c r="M16" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="N16" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="O16" s="9">
+        <v>1154</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -1242,30 +1386,38 @@
       <c r="E17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <v>759</v>
+      <c r="F17" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="3">
+        <v>340</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="11">
-        <v>5424</v>
+        <v>34</v>
+      </c>
+      <c r="M17" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="N17" s="26">
+        <v>16071</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>7</v>
       </c>
@@ -1278,32 +1430,38 @@
       <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="2">
+      <c r="F18" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="3">
         <v>340</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>50</v>
+        <v>34</v>
+      </c>
+      <c r="M18" s="26">
+        <v>1205</v>
+      </c>
+      <c r="N18" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="5">
         <v>8</v>
       </c>
@@ -1316,45 +1474,51 @@
       <c r="E19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="6">
+      <c r="F19" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="5">
         <v>340</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
+      </c>
+      <c r="M19" s="25">
+        <v>1175</v>
+      </c>
+      <c r="N19" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G10:M10"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:O10"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G2:M2"/>
     <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>

</xml_diff>